<commit_message>
Replaced SparkFun Electret microphone with SparkFun MEMS microphone.  Added notes and clarifications to parts list.
</commit_message>
<xml_diff>
--- a/Hardware/PODD_v1.2_PartsList.xlsx
+++ b/Hardware/PODD_v1.2_PartsList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lmnarchitects-my.sharepoint.com/personal/csavage_lmnarchitects_com/Documents/LMN_develop/git/PODD/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="199" documentId="8_{45D655F1-2DAF-434A-B5A7-3E21546DDE12}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{846EFFCA-5B41-410B-B299-CF1DC5647ABE}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{45D655F1-2DAF-434A-B5A7-3E21546DDE12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A4150FCC-94B1-4B48-8401-A6334ABD4DCF}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5940" yWindow="2265" windowWidth="21600" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="162">
   <si>
     <t>Designator</t>
   </si>
@@ -113,9 +113,6 @@
     <t>P1</t>
   </si>
   <si>
-    <t>CMR-2747PB-A</t>
-  </si>
-  <si>
     <t>P8</t>
   </si>
   <si>
@@ -281,9 +278,6 @@
     <t>CO2Meter.com</t>
   </si>
   <si>
-    <t>COZIR-AV-1</t>
-  </si>
-  <si>
     <t>480-5706-1-ND</t>
   </si>
   <si>
@@ -311,9 +305,6 @@
     <t>NTGD1100LT1GOSCT-ND</t>
   </si>
   <si>
-    <t>BOB-12758</t>
-  </si>
-  <si>
     <t>1276-3022-1-ND</t>
   </si>
   <si>
@@ -537,6 +528,18 @@
   </si>
   <si>
     <t>Terminal to face outward from PCB.</t>
+  </si>
+  <si>
+    <t>CozIR-A</t>
+  </si>
+  <si>
+    <t>Used 5,000ppm version (w/o temperature &amp; humidity sensor), but any of the CoZIR-A sensors work.</t>
+  </si>
+  <si>
+    <t>BOB-09868</t>
+  </si>
+  <si>
+    <t>INMP401</t>
   </si>
 </sst>
 </file>
@@ -622,7 +625,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -630,6 +632,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -950,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,142 +987,142 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>130</v>
+        <v>67</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="A2" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="10"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1">
         <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M6" s="1"/>
     </row>
@@ -1137,18 +1140,18 @@
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
@@ -1157,22 +1160,22 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -1181,22 +1184,22 @@
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
@@ -1205,22 +1208,22 @@
         <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
@@ -1232,19 +1235,19 @@
         <v>150</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
@@ -1253,22 +1256,22 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -1280,37 +1283,37 @@
         <v>390</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M14" s="1"/>
     </row>
@@ -1328,36 +1331,36 @@
         <v>12</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="C16" s="1">
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M16" s="1"/>
     </row>
@@ -1375,62 +1378,62 @@
         <v>9</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="A18" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I19" s="1">
         <v>2</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1447,96 +1450,96 @@
         <v>17</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="I20" s="1">
         <v>2</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C21" s="1">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I21" s="1">
         <v>2</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F22" s="1">
         <v>2745</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I22" s="1">
         <v>1</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K22" s="1">
         <v>1014</v>
@@ -1545,34 +1548,34 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="E23" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I23" s="1">
         <v>1</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K23">
         <v>1017</v>
@@ -1580,34 +1583,34 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="E24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="G24" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I24" s="1">
         <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K24" s="1">
         <v>1017</v>
@@ -1615,14 +1618,14 @@
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="A25" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
       <c r="G25" s="3"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1633,34 +1636,34 @@
         <v>18</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>161</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>19</v>
+        <v>161</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I26" s="1">
         <v>1</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K26">
-        <v>1013</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1677,158 +1680,161 @@
         <v>6</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="G27" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I27" s="1">
         <v>1</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K27">
         <v>1012</v>
       </c>
       <c r="M27" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="C28" s="1">
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I28" s="1">
         <v>2</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>75</v>
+        <v>158</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I29" s="1">
         <v>1</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K29">
         <v>1025</v>
       </c>
+      <c r="M29" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I30" s="1">
         <v>1</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="M30" s="1"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="1"/>
@@ -1836,25 +1842,25 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="3"/>
@@ -1863,50 +1869,50 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="M32" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="M32" s="1" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
+      <c r="A33" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1">
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I34" s="1">
+        <v>1</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I34" s="1">
-        <v>1</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="K34" s="1">
         <v>1015</v>
@@ -1915,32 +1921,32 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1">
         <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35" s="1">
+        <v>1</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I35" s="1">
-        <v>1</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="K35">
         <v>1012</v>
@@ -1948,68 +1954,68 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1">
         <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I36" s="1">
+        <v>1</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I36" s="1">
-        <v>1</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="K36" s="1">
         <v>1015</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1">
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I37" s="1">
+        <v>1</v>
+      </c>
+      <c r="J37" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I37" s="1">
-        <v>1</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="K37">
         <v>1013</v>
@@ -2017,121 +2023,121 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="G38" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I38" s="1">
         <v>1</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K38" s="1">
         <v>2494</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="G39" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I39" s="1">
         <v>1</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K39">
         <v>2493</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
+      <c r="A40" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="L41" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
-        <v>147</v>
-      </c>
-      <c r="E41" t="s">
-        <v>66</v>
-      </c>
-      <c r="F41" s="1" t="s">
+      <c r="M41" t="s">
         <v>148</v>
-      </c>
-      <c r="L41" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="M41" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="L42" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="M42" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="M43" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G45" s="11" t="s">
-        <v>156</v>
+      <c r="G45" s="10" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>